<commit_message>
Robot para consulta de cooredenadas de las tiendas
</commit_message>
<xml_diff>
--- a/Sample/Sample/RPA Imagenes.xlsx
+++ b/Sample/Sample/RPA Imagenes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\Archivos MAAJI\Otros\UIPath RPA\Sample\Sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\RPA-UIPATH\Sample\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17499F5-2816-42CB-BA6F-D94EE2BBF087}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1746831C-4466-4CEE-9CD0-781D054A71E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nombre_bottom</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/maaji/image/upload/v1542894279/Spring2019/3007SAC34_3007SBC34_3007SCC34_3007SDC34_WHITE_4.jpg</t>
+  </si>
+  <si>
+    <t>OLIVEIRA FRILLS</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/maaji/image/upload/v1542895401/Spring2019/2110SBC08_2110SCC08_BLUE_1.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/maaji/image/upload/v1542895404/Spring2019/2110SBC08_2110SCC08_BLUE_2.jpg</t>
   </si>
 </sst>
 </file>
@@ -913,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,6 +980,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>